<commit_message>
Stromkabel auf BOM hinzugefügt
</commit_message>
<xml_diff>
--- a/1_Hardware/BOM.xlsx
+++ b/1_Hardware/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows-Massdata\Magellan2\LeapData\Desktop\Projects\OSAMD\OSAMD\1_Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46F8A614-F24C-4CCA-877B-777C1D341E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1750E67B-DCCD-4A73-AF9B-C45C9F8BE879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{EBF05EDD-58DC-4A6B-92AD-20D1351749EB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>BOM: OSAMD-Projekt</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Stromkabel</t>
+  </si>
+  <si>
+    <t>https://de.aliexpress.com/item/4000993209004.html</t>
+  </si>
+  <si>
+    <t>USB zu DC 5,5 * 2,5mm Stromkabel</t>
   </si>
 </sst>
 </file>
@@ -272,13 +281,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -318,8 +327,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70348FC9-2511-44F8-85ED-A54440F619E6}" name="Tabelle1" displayName="Tabelle1" ref="B6:H20" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B6:H20" xr:uid="{3C6EB601-0085-465A-918A-58E43EF5CC0B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70348FC9-2511-44F8-85ED-A54440F619E6}" name="Tabelle1" displayName="Tabelle1" ref="B6:H21" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B6:H21" xr:uid="{3C6EB601-0085-465A-918A-58E43EF5CC0B}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CB3151E0-9214-4D60-9910-29207DEE180A}" name="Teil Nr."/>
     <tableColumn id="5" xr3:uid="{F1816932-E22F-45DC-AC43-BEDAD49DB2BD}" name="Bezeichnung"/>
@@ -630,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55CE553-DF77-4DA6-BCAF-F63786D9F51E}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,78 +655,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -734,10 +743,10 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -754,13 +763,13 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>1.6</v>
       </c>
       <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -777,13 +786,13 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>0.8</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -800,10 +809,10 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>0.5</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -820,13 +829,13 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>0.05</v>
       </c>
       <c r="G11" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -843,13 +852,13 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>0.03</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -866,10 +875,10 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>0.25</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -886,13 +895,13 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>0.1</v>
       </c>
       <c r="G14" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -909,13 +918,13 @@
       <c r="E15">
         <v>2</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>0.01</v>
       </c>
       <c r="G15" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -932,13 +941,13 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>0.01</v>
       </c>
       <c r="G16" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -955,13 +964,13 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>0.01</v>
       </c>
       <c r="G17" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -978,13 +987,13 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>0.01</v>
       </c>
       <c r="G18" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1001,14 +1010,14 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <f>1.69 / 5</f>
         <v>0.33799999999999997</v>
       </c>
       <c r="G19" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1017,33 +1026,53 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
         <v>53</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>54</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F21" s="3">
         <v>4</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>54</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="5">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="4">
         <f>SUM(Tabelle1[Preis])</f>
-        <v>8.7079999999999984</v>
+        <v>9.5380000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1064,11 +1093,12 @@
     <hyperlink ref="H17" r:id="rId11" xr:uid="{3ED3EC20-7B45-4FD2-8940-5A1457099003}"/>
     <hyperlink ref="H18" r:id="rId12" xr:uid="{30548B22-9440-4B5B-851E-8667A6F06125}"/>
     <hyperlink ref="H19" r:id="rId13" xr:uid="{E0181B65-AF56-4ED5-BCE4-E6834D02DD97}"/>
+    <hyperlink ref="H20" r:id="rId14" xr:uid="{33B65EDD-D29E-4703-AF4A-BA30F8FA3299}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Kleine Typingfixes und eine spezifizierung der LED-Position
Danke an @AlexWerz für den Hinweis der ungenauen LED-Beschreibung!

Co-Authored-By: AlexWerz <8876196+AlexWerz@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/1_Hardware/BOM.xlsx
+++ b/1_Hardware/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows-Massdata\Magellan2\LeapData\Desktop\Projects\OSAMD\OSAMD\1_Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1750E67B-DCCD-4A73-AF9B-C45C9F8BE879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52591B4C-105D-4DBC-8FA5-15917BC60E9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{EBF05EDD-58DC-4A6B-92AD-20D1351749EB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>BOM: OSAMD-Projekt</t>
   </si>
@@ -90,9 +90,6 @@
     <t>https://de.aliexpress.com/item/32649621944.html</t>
   </si>
   <si>
-    <t>Es kann auch direkt ausgeählt werden, dass ein I2C-Wandler vorinstalliert werden soll. Dies spart Arbeit und Versandkosten.</t>
-  </si>
-  <si>
     <t>https://de.aliexpress.com/item/32241679858.html</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Preis für 100 Stück circa 3 Euro</t>
   </si>
   <si>
-    <t>Common Anode RGB LED</t>
-  </si>
-  <si>
     <t>Stromanschluss</t>
   </si>
   <si>
@@ -208,6 +202,24 @@
   </si>
   <si>
     <t>USB zu DC 5,5 * 2,5mm Stromkabel</t>
+  </si>
+  <si>
+    <t>Common Anode RGB LED (5mm)</t>
+  </si>
+  <si>
+    <t>Hinweise:</t>
+  </si>
+  <si>
+    <t>Allgemein lohnt es sich, die Teile zu Vergleichen und zu schauen, wer zur Zeit die besten Teilpreise liefert.</t>
+  </si>
+  <si>
+    <t>Auch Sammelbestellungen lohnen sich sehr, so schafft man niedrigere Gesamtpreise und spart Versandkosten und CO2-Emissionen.</t>
+  </si>
+  <si>
+    <t>Es kann auch direkt ausgwählt werden, dass ein I2C-Wandler vorinstalliert werden soll. Dies spart Arbeit und Versandkosten.</t>
+  </si>
+  <si>
+    <t>Es gibt verschiende Längen und unterschiedliche Kabelfarben zur Auswahl, solange der Anschluss passt, ist diese Auswahl egal.</t>
   </si>
 </sst>
 </file>
@@ -639,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55CE553-DF77-4DA6-BCAF-F63786D9F51E}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -767,10 +779,10 @@
         <v>1.6</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -790,7 +802,7 @@
         <v>0.8</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>17</v>
@@ -821,10 +833,10 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -833,10 +845,10 @@
         <v>0.05</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -844,10 +856,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -856,10 +868,10 @@
         <v>0.03</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -867,10 +879,10 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -879,7 +891,7 @@
         <v>0.25</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -887,10 +899,10 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -899,10 +911,10 @@
         <v>0.1</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -910,10 +922,10 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -922,10 +934,10 @@
         <v>0.01</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -933,10 +945,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -945,10 +957,10 @@
         <v>0.01</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -956,10 +968,10 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -968,10 +980,10 @@
         <v>0.01</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -979,10 +991,10 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -991,10 +1003,10 @@
         <v>0.01</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1002,10 +1014,10 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1015,10 +1027,10 @@
         <v>0.33799999999999997</v>
       </c>
       <c r="G19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1026,10 +1038,10 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
         <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1037,8 +1049,11 @@
       <c r="F20" s="3">
         <v>0.83</v>
       </c>
+      <c r="G20" t="s">
+        <v>61</v>
+      </c>
       <c r="H20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1046,33 +1061,46 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F21" s="3">
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="4">
         <f>SUM(Tabelle1[Preis])</f>
         <v>9.5380000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>